<commit_message>
change columns in sensor data
</commit_message>
<xml_diff>
--- a/global_variable_template_new.xlsx
+++ b/global_variable_template_new.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="15120" windowHeight="14220"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="15120" windowHeight="14220" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="399">
   <si>
     <t>[3(FALSE)]</t>
   </si>
@@ -1293,7 +1293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1311,6 +1311,9 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1593,8 +1596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2920,100 +2923,129 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>25</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2">
+      <c r="C2" s="9">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>26</v>
       </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3">
+      <c r="C3" s="9">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3">
         <v>0</v>
       </c>
+      <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>29</v>
       </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4">
+      <c r="C4" s="9">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>27</v>
       </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5">
+      <c r="C5" s="9">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>28</v>
       </c>
-      <c r="B6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6">
+      <c r="C6" s="9">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
         <v>30</v>
       </c>
-      <c r="B7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7">
+      <c r="C7" s="9">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C8" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
edit code to read updated table
</commit_message>
<xml_diff>
--- a/global_variable_template_new.xlsx
+++ b/global_variable_template_new.xlsx
@@ -2366,7 +2366,7 @@
   <dimension ref="A1:C103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2926,7 +2926,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2960,6 +2960,9 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>12000</v>
+      </c>
       <c r="B2" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
update sensor base addr
</commit_message>
<xml_diff>
--- a/global_variable_template_new.xlsx
+++ b/global_variable_template_new.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="400">
   <si>
     <t>[3(FALSE)]</t>
   </si>
@@ -1233,6 +1233,9 @@
   </si>
   <si>
     <t>DUMMY_BIT_FALSE</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -2926,7 +2929,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2960,8 +2963,8 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>12000</v>
+      <c r="A2" t="s">
+        <v>399</v>
       </c>
       <c r="B2" t="s">
         <v>25</v>

</xml_diff>